<commit_message>
Zeiterfassung_Kasper_Christian.xlsx: Erfassung von gestern + kleinere Korikturen
</commit_message>
<xml_diff>
--- a/1. Projektplanung und Dokumentation/1.1 Zeiterfassung/Zeiterfassung_Kasper_Christian.xlsx
+++ b/1. Projektplanung und Dokumentation/1.1 Zeiterfassung/Zeiterfassung_Kasper_Christian.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thude0-my.sharepoint.com/personal/kaspch01_hs-ulm_de/Documents/Semester 5/Software Projekt/RaytRazor/RaytRazor/1. Projektplanung/1.1 Zeiterfassung/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thude0-my.sharepoint.com/personal/kaspch01_hs-ulm_de/Documents/Semester 5/Software Projekt/RaytRazor/RaytRazor/1. Projektplanung und Dokumentation/1.1 Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{94D13F69-E4BB-4FA5-BDE2-F9BADDE19940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43A4CECB-8802-4B4C-806D-96F722FA298C}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{94D13F69-E4BB-4FA5-BDE2-F9BADDE19940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5F190ED-C88A-4B8B-8D67-3D5B98347835}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="38610" windowHeight="20985" xr2:uid="{A62B9331-51AB-445E-8A86-E52DCE8B38AE}"/>
+    <workbookView xWindow="29655" yWindow="2370" windowWidth="21075" windowHeight="15345" xr2:uid="{A62B9331-51AB-445E-8A86-E52DCE8B38AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeiterfassung" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
   <si>
     <t>Name:</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>Erfahrungsbericht + Lastenheft + letzte Buggs in GUI</t>
+  </si>
+  <si>
+    <t>Lastenheft und GUI</t>
   </si>
 </sst>
 </file>
@@ -493,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{709269E3-F8C7-4951-A5F4-E55A0F95233D}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -554,8 +557,8 @@
         <v>9</v>
       </c>
       <c r="F6">
-        <f>SUM(B7:B31)</f>
-        <v>114.15</v>
+        <f>SUM(B7:B32)</f>
+        <v>137.15</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -633,7 +636,7 @@
         <v>45588</v>
       </c>
       <c r="B12" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
@@ -787,7 +790,7 @@
         <v>45638</v>
       </c>
       <c r="B23" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C23" t="s">
         <v>21</v>
@@ -815,7 +818,7 @@
         <v>45671</v>
       </c>
       <c r="B25" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C25" t="s">
         <v>17</v>
@@ -857,7 +860,7 @@
         <v>45674</v>
       </c>
       <c r="B28" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C28" t="s">
         <v>17</v>
@@ -899,13 +902,27 @@
         <v>45677</v>
       </c>
       <c r="B31" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C31" t="s">
         <v>17</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="4">
+        <v>45678</v>
+      </c>
+      <c r="B32" s="2">
+        <v>13</v>
+      </c>
+      <c r="C32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1061,18 +1078,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1094,18 +1111,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C634F9CB-9B15-47F9-9574-21334E2C6303}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2314BDC-9EA2-4E30-A7C5-448E8CFAD4C2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C634F9CB-9B15-47F9-9574-21334E2C6303}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>